<commit_message>
Fix: Error en el ingreso de la fecha
</commit_message>
<xml_diff>
--- a/facturacion.xlsx
+++ b/facturacion.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\facturaElectronicaPy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1856B09F-62A0-470A-95E8-13BA5F9379D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3CF282D-79AC-4F6D-8403-BE47801B016B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,21 +16,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -43,64 +29,64 @@
     <t>TIPO_FACTURA</t>
   </si>
   <si>
+    <t>TIPO_DOCUMENTO</t>
+  </si>
+  <si>
+    <t>NUMERO_DOC</t>
+  </si>
+  <si>
     <t>MEDIO_PAGO</t>
   </si>
   <si>
+    <t>TIPO_TARJETA</t>
+  </si>
+  <si>
     <t>PRECIO</t>
   </si>
   <si>
-    <t>TIPO_DOCUMENTO</t>
-  </si>
-  <si>
-    <t>NUMERO_DOC</t>
+    <t>ESTADO</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>DNI</t>
+  </si>
+  <si>
+    <t>DEBITO</t>
+  </si>
+  <si>
+    <t>MASTERCARD</t>
+  </si>
+  <si>
+    <t>PASO</t>
+  </si>
+  <si>
+    <t>VISA</t>
+  </si>
+  <si>
+    <t>CREDITO</t>
+  </si>
+  <si>
+    <t>TIPO_DOC</t>
   </si>
   <si>
     <t>CUIT</t>
   </si>
   <si>
+    <t>QR</t>
+  </si>
+  <si>
     <t>CUIL</t>
   </si>
   <si>
-    <t>DNI</t>
-  </si>
-  <si>
-    <t>QR</t>
-  </si>
-  <si>
     <t>EFECTIVO</t>
   </si>
   <si>
-    <t>DEBITO</t>
-  </si>
-  <si>
-    <t>CREDITO</t>
-  </si>
-  <si>
-    <t>TIPO_DOC</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>TIPO_TARJETA</t>
-  </si>
-  <si>
-    <t>VISA</t>
-  </si>
-  <si>
-    <t>MASTERCARD</t>
-  </si>
-  <si>
     <t>COBOL</t>
   </si>
   <si>
     <t>NARANJA</t>
-  </si>
-  <si>
-    <t>ESTADO</t>
-  </si>
-  <si>
-    <t>PASO</t>
   </si>
 </sst>
 </file>
@@ -108,27 +94,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -154,7 +126,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -178,17 +150,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -348,52 +309,48 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="12">
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      <border>
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -415,8 +372,8 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -430,7 +387,7 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      <border>
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -446,7 +403,7 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      <border>
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -468,7 +425,7 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      <border>
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -490,7 +447,7 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      <border>
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -512,7 +469,7 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      <border>
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -535,7 +492,7 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border>
         <left/>
         <right style="thin">
           <color indexed="64"/>
@@ -562,7 +519,7 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      <border>
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -585,8 +542,8 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="center" vertical="center"/>
+      <border>
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -615,17 +572,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4E75E09A-9B4E-4D7D-9B29-1D9D51840EC6}" name="Tabla2" displayName="Tabla2" ref="A1:H42" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
-  <autoFilter ref="A1:H42" xr:uid="{4E75E09A-9B4E-4D7D-9B29-1D9D51840EC6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla2" displayName="Tabla2" ref="A1:H42" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+  <autoFilter ref="A1:H42" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{47D862BA-761E-499B-8289-85A03BE14C44}" name="FECHA" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{14CB85AF-32F9-476A-BA0F-0D61B1FC1AAB}" name="TIPO_FACTURA" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{E2063639-BAF4-4469-BD7C-F6C0E7CAC213}" name="TIPO_DOCUMENTO" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{1C596E7B-B865-4A22-A143-2FB45B674FFA}" name="NUMERO_DOC" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{AF9FA0C5-3B2E-490F-8A8B-B812197EB318}" name="MEDIO_PAGO" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{7D3E8BE4-1837-4F71-AD76-8B35289EFCEE}" name="TIPO_TARJETA" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{49904E19-348B-4915-BF87-76A20FC68924}" name="PRECIO" dataDxfId="1"/>
-    <tableColumn id="12" xr3:uid="{1E11A149-2E92-4E28-A627-29F70E06CDA9}" name="ESTADO" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="FECHA" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="TIPO_FACTURA" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="TIPO_DOCUMENTO" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="NUMERO_DOC" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="MEDIO_PAGO" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="TIPO_TARJETA" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="PRECIO" dataDxfId="1"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="ESTADO" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -897,10 +854,10 @@
   <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="18.7109375" customWidth="1"/>
@@ -912,7 +869,7 @@
     <col min="9" max="9" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -920,489 +877,452 @@
         <v>1</v>
       </c>
       <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="F1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="22" t="s">
-        <v>20</v>
+      <c r="G1" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="20"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="17"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
+      <c r="A3" s="11"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="15"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="18"/>
       <c r="H3" s="19"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
+      <c r="A4" s="11"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="3"/>
       <c r="F4" s="3"/>
-      <c r="G4" s="15"/>
+      <c r="G4" s="18"/>
       <c r="H4" s="19"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="25"/>
+      <c r="A5" s="11"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="3"/>
-      <c r="G5" s="15"/>
+      <c r="G5" s="16"/>
       <c r="H5" s="19"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
+      <c r="A6" s="11"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="E6" s="6"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="15"/>
+      <c r="G6" s="16"/>
       <c r="H6" s="19"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
+      <c r="A7" s="11"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="E7" s="6"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="15"/>
+      <c r="G7" s="16"/>
       <c r="H7" s="19"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
+      <c r="A8" s="11"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="24"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="19"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
+      <c r="A9" s="11"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="15"/>
+      <c r="G9" s="16"/>
       <c r="H9" s="19"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
+      <c r="A10" s="11"/>
       <c r="B10" s="2"/>
-      <c r="C10" s="17"/>
+      <c r="C10" s="2"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="E10" s="6"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="15"/>
+      <c r="G10" s="16"/>
       <c r="H10" s="19"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
+      <c r="A11" s="11"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="E11" s="6"/>
       <c r="F11" s="3"/>
-      <c r="G11" s="15"/>
+      <c r="G11" s="16"/>
       <c r="H11" s="19"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
+      <c r="A12" s="11"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="E12" s="6"/>
       <c r="F12" s="3"/>
-      <c r="G12" s="15"/>
+      <c r="G12" s="16"/>
       <c r="H12" s="19"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
+      <c r="A13" s="11"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="E13" s="6"/>
       <c r="F13" s="3"/>
-      <c r="G13" s="15"/>
+      <c r="G13" s="16"/>
       <c r="H13" s="19"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
+      <c r="A14" s="11"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="E14" s="6"/>
       <c r="F14" s="3"/>
-      <c r="G14" s="15"/>
+      <c r="G14" s="16"/>
       <c r="H14" s="19"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
+      <c r="A15" s="11"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+      <c r="E15" s="6"/>
       <c r="F15" s="3"/>
-      <c r="G15" s="15"/>
+      <c r="G15" s="16"/>
       <c r="H15" s="19"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
+      <c r="A16" s="11"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="3"/>
-      <c r="G16" s="15"/>
+      <c r="G16" s="16"/>
       <c r="H16" s="19"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
+      <c r="A17" s="11"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="3"/>
-      <c r="G17" s="15"/>
+      <c r="G17" s="16"/>
       <c r="H17" s="19"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
+      <c r="A18" s="11"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="3"/>
-      <c r="G18" s="15"/>
+      <c r="G18" s="16"/>
       <c r="H18" s="19"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
+      <c r="A19" s="11"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+      <c r="E19" s="6"/>
       <c r="F19" s="3"/>
-      <c r="G19" s="15"/>
+      <c r="G19" s="16"/>
       <c r="H19" s="19"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="12"/>
+      <c r="A20" s="11"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="3"/>
-      <c r="G20" s="15"/>
+      <c r="G20" s="16"/>
       <c r="H20" s="19"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
+      <c r="A21" s="11"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="3"/>
-      <c r="G21" s="15"/>
+      <c r="G21" s="16"/>
       <c r="H21" s="19"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
+      <c r="A22" s="11"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="3"/>
-      <c r="G22" s="15"/>
+      <c r="G22" s="16"/>
       <c r="H22" s="19"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
+      <c r="A23" s="11"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="3"/>
-      <c r="G23" s="15"/>
+      <c r="G23" s="16"/>
       <c r="H23" s="19"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="12"/>
+      <c r="A24" s="11"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="3"/>
-      <c r="G24" s="15"/>
+      <c r="G24" s="16"/>
       <c r="H24" s="19"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="12"/>
+      <c r="A25" s="11"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="3"/>
-      <c r="G25" s="15"/>
+      <c r="G25" s="16"/>
       <c r="H25" s="19"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="12"/>
+      <c r="A26" s="11"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="3"/>
-      <c r="G26" s="15"/>
+      <c r="G26" s="16"/>
       <c r="H26" s="19"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="12"/>
+      <c r="A27" s="11"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="3"/>
-      <c r="G27" s="15"/>
+      <c r="G27" s="16"/>
       <c r="H27" s="19"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="12"/>
+      <c r="A28" s="11"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="3"/>
-      <c r="G28" s="15"/>
+      <c r="G28" s="16"/>
       <c r="H28" s="19"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="12"/>
+      <c r="A29" s="11"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="3"/>
-      <c r="G29" s="15"/>
+      <c r="G29" s="16"/>
       <c r="H29" s="19"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
+      <c r="A30" s="11"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="3"/>
-      <c r="G30" s="15"/>
+      <c r="G30" s="16"/>
       <c r="H30" s="19"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="12"/>
+      <c r="A31" s="11"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="3"/>
-      <c r="G31" s="15"/>
+      <c r="G31" s="16"/>
       <c r="H31" s="19"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="12"/>
+      <c r="A32" s="11"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="3"/>
-      <c r="G32" s="15"/>
+      <c r="G32" s="16"/>
       <c r="H32" s="19"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="12"/>
+      <c r="A33" s="11"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="3"/>
-      <c r="G33" s="15"/>
+      <c r="G33" s="16"/>
       <c r="H33" s="19"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="12"/>
+      <c r="A34" s="11"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="3"/>
-      <c r="G34" s="15"/>
+      <c r="G34" s="16"/>
       <c r="H34" s="19"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="12"/>
+      <c r="A35" s="11"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="3"/>
-      <c r="G35" s="15"/>
+      <c r="G35" s="16"/>
       <c r="H35" s="19"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="12"/>
+      <c r="A36" s="11"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="3"/>
-      <c r="G36" s="15"/>
+      <c r="G36" s="16"/>
       <c r="H36" s="19"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="12"/>
+      <c r="A37" s="11"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="3"/>
-      <c r="G37" s="15"/>
+      <c r="G37" s="16"/>
       <c r="H37" s="19"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="12"/>
+      <c r="A38" s="11"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
       <c r="F38" s="3"/>
-      <c r="G38" s="15"/>
+      <c r="G38" s="16"/>
       <c r="H38" s="19"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="12"/>
+      <c r="A39" s="11"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
       <c r="F39" s="3"/>
-      <c r="G39" s="15"/>
+      <c r="G39" s="16"/>
       <c r="H39" s="19"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="12"/>
+      <c r="A40" s="11"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
       <c r="F40" s="3"/>
-      <c r="G40" s="15"/>
+      <c r="G40" s="16"/>
       <c r="H40" s="19"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="12"/>
+      <c r="A41" s="11"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
       <c r="F41" s="3"/>
-      <c r="G41" s="15"/>
+      <c r="G41" s="16"/>
       <c r="H41" s="19"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="13"/>
+      <c r="A42" s="12"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
       <c r="F42" s="5"/>
-      <c r="G42" s="16"/>
+      <c r="G42" s="20"/>
       <c r="H42" s="21"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6F7852A4-CAB2-41E0-96D3-1FA3B3221AA9}">
-          <x14:formula1>
-            <xm:f>Hoja2!$A$4:$A$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>C1:C1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{82041B52-2D69-48B5-B6EC-5B7DBA0F342C}">
-          <x14:formula1>
-            <xm:f>Hoja2!$B$4:$B$7</xm:f>
-          </x14:formula1>
-          <xm:sqref>E2:E28</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{87B89C28-4826-48B0-8393-215D7CFDAA62}">
-          <x14:formula1>
-            <xm:f>Hoja2!$C$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>B1:B1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{35DC8074-529A-4AB3-9BF2-B0B437101DC2}">
-          <x14:formula1>
-            <xm:f>Hoja2!$D$4:$D$7</xm:f>
-          </x14:formula1>
-          <xm:sqref>F1:F1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A19ADC35-8E5E-4710-977B-7F0284584CCB}">
-          <x14:formula1>
-            <xm:f>Hoja2!$E$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>H1:H1048576</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22874AA4-9D6A-4455-9837-E38A68C09F2A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A3:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.140625" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" customWidth="1"/>
@@ -1411,66 +1331,66 @@
   <sheetData>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>